<commit_message>
type split calibration - i think its good enough now
</commit_message>
<xml_diff>
--- a/Data/cleaned_and_combined_data/Type_Split/type_split_clean.xlsx
+++ b/Data/cleaned_and_combined_data/Type_Split/type_split_clean.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/954e9104582efe7e/Documents/Python/TEP4290_project/data/cleaned_and_combined_data/Type_Split/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{17722BCC-DBE4-41E7-9468-88373FB63645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9359BA73-E25C-4F1E-B1E9-7F9B48DD9E85}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{17722BCC-DBE4-41E7-9468-88373FB63645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51AA440E-6935-4B6F-88E8-CD23B4FDF661}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{819B9427-967E-4C73-814F-69767B50FEA4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{819B9427-967E-4C73-814F-69767B50FEA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
   <si>
     <t>Age classes</t>
   </si>
@@ -615,11 +616,11 @@
       </c>
       <c r="B2" s="1">
         <f>1-C2</f>
-        <v>0.99333333333333329</v>
+        <v>0.9906666666666667</v>
       </c>
       <c r="C2" s="1">
-        <f>0.02*2/3*0.5</f>
-        <v>6.6666666666666671E-3</v>
+        <f>0.02*2/3*0.5*1.4</f>
+        <v>9.3333333333333341E-3</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -631,14 +632,15 @@
       </c>
       <c r="B3" s="1">
         <f>1-C3-D3</f>
-        <v>0.68606232286796176</v>
+        <v>0.70930177018149099</v>
       </c>
       <c r="C3" s="1">
-        <f>0.197740440564393*2/3*0.5</f>
-        <v>6.5913480188130993E-2</v>
+        <f>0.197740440564393*2/3*0.5*1.4</f>
+        <v>9.2278872263383382E-2</v>
       </c>
       <c r="D3" s="1">
-        <v>0.2480241969439072</v>
+        <f>0.248024196943907*0.8</f>
+        <v>0.19841935755512563</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -647,14 +649,15 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:B9" si="0">1-C4-D4</f>
-        <v>0.65522686199512292</v>
+        <v>0.68631478455692085</v>
       </c>
       <c r="C4" s="1">
-        <f>0.189333525195886*2/3*0.5</f>
-        <v>6.311117506529533E-2</v>
+        <f>0.189333525195886*2/3*0.5*1.4</f>
+        <v>8.8355645091413457E-2</v>
       </c>
       <c r="D4" s="1">
-        <v>0.28166196293958179</v>
+        <f>0.281661962939582*0.8</f>
+        <v>0.22532957035166562</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -663,14 +666,15 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
-        <v>0.69873203660591454</v>
+        <v>0.72117301604267814</v>
       </c>
       <c r="C5" s="1">
-        <f>0.189063066210266*2/3*0.5</f>
-        <v>6.3021022070088667E-2</v>
+        <f>0.189063066210266*2/3*0.5*1.4</f>
+        <v>8.8229430898124128E-2</v>
       </c>
       <c r="D5" s="1">
-        <v>0.23824694132399679</v>
+        <f>0.238246941323997*0.8</f>
+        <v>0.19059755305919762</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -679,14 +683,15 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>0.75474946364816109</v>
+        <v>0.72911526468433407</v>
       </c>
       <c r="C6" s="1">
-        <f>0.213790952960481*2/3*0.5</f>
-        <v>7.1263650986827007E-2</v>
+        <f>0.213790952960481*2/3*0.5*1.1*1.2*1.4</f>
+        <v>0.13169522702365632</v>
       </c>
       <c r="D6" s="1">
-        <v>0.17398688536501189</v>
+        <f>0.173986885365012*0.8</f>
+        <v>0.1391895082920096</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -695,14 +700,15 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>0.63712757830404898</v>
+        <v>0.65013820404194722</v>
       </c>
       <c r="C7" s="1">
-        <f>0.241475102437669*2/3*0.5</f>
-        <v>8.0491700812556341E-2</v>
+        <f>0.241475102437669*2/3*0.5*1.1*1.4</f>
+        <v>0.12395721925133676</v>
       </c>
       <c r="D7" s="1">
-        <v>0.28238072088339472</v>
+        <f>0.282380720883395*0.8</f>
+        <v>0.22590457670671601</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -711,15 +717,15 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>0.43848192669795388</v>
+        <v>0.33669662505211706</v>
       </c>
       <c r="C8" s="1">
         <f>0.23047848210847*2/3*0.5</f>
         <v>7.6826160702823332E-2</v>
       </c>
       <c r="D8" s="1">
-        <f>0.432760636249306*1.12</f>
-        <v>0.48469191259922279</v>
+        <f>0.432760636249306*1.12*1.1*1.1</f>
+        <v>0.58647721424505961</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -728,15 +734,15 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>0.45580393481081238</v>
+        <v>0.35885139069081295</v>
       </c>
       <c r="C9" s="1">
         <f>0.247551850996143*2/3*0.5</f>
         <v>8.2517283665380997E-2</v>
       </c>
       <c r="D9" s="1">
-        <f>0.412213197789113*1.12</f>
-        <v>0.46167878152380659</v>
+        <f>0.412213197789113*1.12*1.1*1.1</f>
+        <v>0.55863132564380602</v>
       </c>
     </row>
   </sheetData>
@@ -748,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53CF209A-A198-44F6-BBA1-97A81A1183BF}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -883,4 +889,145 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85770CE1-6A5F-49E6-B3AE-56641D93A0C2}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.9906666666666667</v>
+      </c>
+      <c r="C2" s="1">
+        <v>9.3333333333333341E-3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.70930177018149099</v>
+      </c>
+      <c r="C3" s="1">
+        <v>9.2278872263383382E-2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.19841935755512563</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.68631478455692085</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8.8355645091413457E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.22532957035166562</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.72117301604267814</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8.8229430898124128E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.19059755305919762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.72911526468433407</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.13169522702365632</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.1391895082920096</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.65013820404194722</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.12395721925133676</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.22590457670671601</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.33669662505211706</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7.6826160702823332E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.58647721424505961</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.35885139069081295</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8.2517283665380997E-2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.55863132564380602</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>